<commit_message>
Fix a bug & Add user_to_user
</commit_message>
<xml_diff>
--- a/ooxx.xlsx
+++ b/ooxx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linyuxiang/Desktop/TOC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linyuxiang/Desktop/TOC/project/Chat_Robot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FA0CB5-224B-A341-BE78-C8978C4DDB65}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5747F5-2597-AE4A-A1EA-BD66577348C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="460" windowWidth="25200" windowHeight="16080" activeTab="3" xr2:uid="{70AFC525-7F52-FC42-98BD-6E477B5EE7AA}"/>
+    <workbookView xWindow="3320" yWindow="460" windowWidth="25200" windowHeight="16080" xr2:uid="{70AFC525-7F52-FC42-98BD-6E477B5EE7AA}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1220,9 +1220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAA0581-2072-0449-BF1D-6D6EC0401991}">
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K102" sqref="K102"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100:I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9469,8 +9469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF3835D-B3B8-1040-AC2F-5F53ED9A4242}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I60"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>